<commit_message>
last commit, I hope
</commit_message>
<xml_diff>
--- a/Assignment1-guess-number/Iteration3/document/time_log.xlsx
+++ b/Assignment1-guess-number/Iteration3/document/time_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shukebeta/OneDrive - Ara Institute of Canterbury/BCPR280/Assignment1-guess-number/Iteration3/document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{9B27C467-49CD-DB42-B39F-B8AE1ACF5BEC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{44FF5FC5-5B22-5145-9ABD-B5093BE387BC}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="8_{9B27C467-49CD-DB42-B39F-B8AE1ACF5BEC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{F492FBF2-2653-0043-BDF0-46A2573C1D13}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="14360" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -372,7 +372,7 @@
     <t>Amitrajit Sarkar</t>
   </si>
   <si>
-    <t>BCPR280-Iteration2</t>
+    <t>BCPR280-Iteration3</t>
   </si>
 </sst>
 </file>
@@ -987,7 +987,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>